<commit_message>
Added frontend code for visits with guests.
</commit_message>
<xml_diff>
--- a/storage/timetable.xlsx
+++ b/storage/timetable.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -457,9 +457,295 @@
         <v>3.10.2020, 15:55:16</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>salexandru</v>
+      </c>
+      <c r="B8" t="str">
+        <v>3.10.2020, 16:57:24</v>
+      </c>
+      <c r="C8" t="str">
+        <v>3.10.2020, 16:57:26</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B9" t="str">
+        <v>3.10.2020, 20:8:40</v>
+      </c>
+      <c r="C9" t="str">
+        <v>3.10.2020, 20:9:43</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B10" t="str">
+        <v>3.10.2020, 20:23:30</v>
+      </c>
+      <c r="C10" t="str">
+        <v>3.10.2020, 20:23:44</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B11" t="str">
+        <v>3.10.2020, 20:23:50</v>
+      </c>
+      <c r="C11" t="str">
+        <v>3.10.2020, 20:23:53</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B12" t="str">
+        <v>3.10.2020, 20:52:52</v>
+      </c>
+      <c r="C12" t="str">
+        <v>3.10.2020, 20:56:53</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B13" t="str">
+        <v>3.10.2020, 20:57:48</v>
+      </c>
+      <c r="C13" t="str">
+        <v>3.10.2020, 20:57:51</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B14" t="str">
+        <v>3.10.2020, 20:57:53</v>
+      </c>
+      <c r="C14" t="str">
+        <v>3.10.2020, 20:58:4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B15" t="str">
+        <v>3.10.2020, 20:58:9</v>
+      </c>
+      <c r="C15" t="str">
+        <v>3.10.2020, 20:58:29</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B16" t="str">
+        <v>3.10.2020, 21:9:32</v>
+      </c>
+      <c r="C16" t="str">
+        <v>3.10.2020, 21:9:49</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B17" t="str">
+        <v>3.10.2020, 21:10:8</v>
+      </c>
+      <c r="C17" t="str">
+        <v>3.10.2020, 21:10:10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B18" t="str">
+        <v>3.10.2020, 21:11:4</v>
+      </c>
+      <c r="C18" t="str">
+        <v>3.10.2020, 21:11:6</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B19" t="str">
+        <v>3.10.2020, 21:11:25</v>
+      </c>
+      <c r="C19" t="str">
+        <v>3.10.2020, 21:11:26</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B20" t="str">
+        <v>3.10.2020, 21:11:36</v>
+      </c>
+      <c r="C20" t="str">
+        <v>3.10.2020, 21:11:37</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B21" t="str">
+        <v>3.10.2020, 21:14:1</v>
+      </c>
+      <c r="C21" t="str">
+        <v>3.10.2020, 21:15:4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B22" t="str">
+        <v>3.10.2020, 21:16:8</v>
+      </c>
+      <c r="C22" t="str">
+        <v>3.10.2020, 21:16:13</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B23" t="str">
+        <v>3.10.2020, 21:16:24</v>
+      </c>
+      <c r="C23" t="str">
+        <v>3.10.2020, 21:16:34</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B24" t="str">
+        <v>3.10.2020, 21:16:37</v>
+      </c>
+      <c r="C24" t="str">
+        <v>3.10.2020, 21:16:41</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B25" t="str">
+        <v>3.10.2020, 21:17:8</v>
+      </c>
+      <c r="C25" t="str">
+        <v>3.10.2020, 21:17:12</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B26" t="str">
+        <v>3.10.2020, 21:18:16</v>
+      </c>
+      <c r="C26" t="str">
+        <v>3.10.2020, 21:19:0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B27" t="str">
+        <v>3.10.2020, 21:19:5</v>
+      </c>
+      <c r="C27" t="str">
+        <v>3.10.2020, 21:20:10</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B28" t="str">
+        <v>3.10.2020, 21:20:20</v>
+      </c>
+      <c r="C28" t="str">
+        <v>3.10.2020, 21:21:3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>jane01 (cu dwawdd)</v>
+      </c>
+      <c r="B29" t="str">
+        <v>3.10.2020, 21:21:12</v>
+      </c>
+      <c r="C29" t="str">
+        <v>3.10.2020, 21:23:27</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>jane01 (cu ddd)</v>
+      </c>
+      <c r="B30" t="str">
+        <v>3.10.2020, 21:23:30</v>
+      </c>
+      <c r="C30" t="str">
+        <v>3.10.2020, 21:23:35</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B31" t="str">
+        <v>3.10.2020, 21:23:52</v>
+      </c>
+      <c r="C31" t="str">
+        <v>3.10.2020, 21:23:57</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>jane01</v>
+      </c>
+      <c r="B32" t="str">
+        <v>3.10.2020, 21:27:1</v>
+      </c>
+      <c r="C32" t="str">
+        <v>3.10.2020, 21:28:9</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>salexandru (cu Alex)</v>
+      </c>
+      <c r="B33" t="str">
+        <v>3.10.2020, 21:27:18</v>
+      </c>
+      <c r="C33" t="str">
+        <v>3.10.2020, 21:27:28</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C33"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update gitgnore to remove sensible data
</commit_message>
<xml_diff>
--- a/storage/timetable.xlsx
+++ b/storage/timetable.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -393,359 +393,150 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>salexandru</v>
+        <v>Tudor Avram</v>
       </c>
       <c r="B2" t="str">
-        <v>2.10.2020, 19:15:14</v>
+        <v>3.10.2020, 21:58:55</v>
       </c>
       <c r="C2" t="str">
-        <v>2.10.2020, 19:15:19</v>
+        <v>3.10.2020, 21:59:18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>salexandru</v>
+        <v>Alexandru Sandulescu</v>
       </c>
       <c r="B3" t="str">
-        <v>2.10.2020, 19:15:20</v>
+        <v>3.10.2020, 22:00:22</v>
       </c>
       <c r="C3" t="str">
-        <v>2.10.2020, 19:15:36</v>
+        <v>3.10.2020, 22:00:33</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>salexandru</v>
+        <v>Tudor Avram (cu Alex)</v>
       </c>
       <c r="B4" t="str">
-        <v>2.10.2020, 19:31:10</v>
+        <v>3.10.2020, 22:01:41</v>
       </c>
       <c r="C4" t="str">
-        <v>2.10.2020, 19:31:18</v>
+        <v>3.10.2020, 22:01:45</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>salexandru</v>
+        <v>Alexandru Sandulescu</v>
       </c>
       <c r="B5" t="str">
-        <v>2.10.2020, 19:44:34</v>
+        <v>3.10.2020, 22:04:19</v>
       </c>
       <c r="C5" t="str">
-        <v>2.10.2020, 19:44:47</v>
+        <v>3.10.2020, 22:04:26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>salexandru</v>
+        <v>Alexandru Sandulescu</v>
       </c>
       <c r="B6" t="str">
-        <v>3.10.2020, 15:47:55</v>
+        <v>3.10.2020, 22:04:32</v>
       </c>
       <c r="C6" t="str">
-        <v>3.10.2020, 15:55:13</v>
+        <v>3.10.2020, 22:06:48</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>salexandru</v>
+        <v>Alexandru Sandulescu (cu Sorana Sandulescu)</v>
       </c>
       <c r="B7" t="str">
-        <v>3.10.2020, 15:55:14</v>
+        <v>3.10.2020, 22:07:36</v>
       </c>
       <c r="C7" t="str">
-        <v>3.10.2020, 15:55:16</v>
+        <v>3.10.2020, 22:09:08</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>salexandru</v>
+        <v>Sebastian Georgescu</v>
       </c>
       <c r="B8" t="str">
-        <v>3.10.2020, 16:57:24</v>
+        <v>3.10.2020, 23:27:04</v>
       </c>
       <c r="C8" t="str">
-        <v>3.10.2020, 16:57:26</v>
+        <v>3.10.2020, 23:27:14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>jane01</v>
+        <v>Alexandru Sandulescu</v>
       </c>
       <c r="B9" t="str">
-        <v>3.10.2020, 20:8:40</v>
+        <v>6.10.2020, 19:28:24</v>
       </c>
       <c r="C9" t="str">
-        <v>3.10.2020, 20:9:43</v>
+        <v>6.10.2020, 19:28:32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>jane01</v>
+        <v>Alexandru Sandulescu (cu Sorana)</v>
       </c>
       <c r="B10" t="str">
-        <v>3.10.2020, 20:23:30</v>
+        <v>6.10.2020, 19:28:37</v>
       </c>
       <c r="C10" t="str">
-        <v>3.10.2020, 20:23:44</v>
+        <v>6.10.2020, 19:28:48</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>jane01</v>
+        <v>Alexandru Sandulescu</v>
       </c>
       <c r="B11" t="str">
-        <v>3.10.2020, 20:23:50</v>
+        <v>6.10.2020, 19:33:03</v>
       </c>
       <c r="C11" t="str">
-        <v>3.10.2020, 20:23:53</v>
+        <v>6.10.2020, 19:33:19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>jane01</v>
+        <v>Alexandru Sandulescu (cu d)</v>
       </c>
       <c r="B12" t="str">
-        <v>3.10.2020, 20:52:52</v>
+        <v>6.10.2020, 19:42:54</v>
       </c>
       <c r="C12" t="str">
-        <v>3.10.2020, 20:56:53</v>
+        <v>6.10.2020, 19:43:01</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>jane01</v>
+        <v>Alexandru Sandulescu</v>
       </c>
       <c r="B13" t="str">
-        <v>3.10.2020, 20:57:48</v>
+        <v>6.10.2020, 19:47:01</v>
       </c>
       <c r="C13" t="str">
-        <v>3.10.2020, 20:57:51</v>
+        <v>6.10.2020, 19:47:22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>jane01</v>
+        <v>Alexandru Sandulescu</v>
       </c>
       <c r="B14" t="str">
-        <v>3.10.2020, 20:57:53</v>
+        <v>6.10.2020, 20:11:43</v>
       </c>
       <c r="C14" t="str">
-        <v>3.10.2020, 20:58:4</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B15" t="str">
-        <v>3.10.2020, 20:58:9</v>
-      </c>
-      <c r="C15" t="str">
-        <v>3.10.2020, 20:58:29</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B16" t="str">
-        <v>3.10.2020, 21:9:32</v>
-      </c>
-      <c r="C16" t="str">
-        <v>3.10.2020, 21:9:49</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B17" t="str">
-        <v>3.10.2020, 21:10:8</v>
-      </c>
-      <c r="C17" t="str">
-        <v>3.10.2020, 21:10:10</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B18" t="str">
-        <v>3.10.2020, 21:11:4</v>
-      </c>
-      <c r="C18" t="str">
-        <v>3.10.2020, 21:11:6</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B19" t="str">
-        <v>3.10.2020, 21:11:25</v>
-      </c>
-      <c r="C19" t="str">
-        <v>3.10.2020, 21:11:26</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B20" t="str">
-        <v>3.10.2020, 21:11:36</v>
-      </c>
-      <c r="C20" t="str">
-        <v>3.10.2020, 21:11:37</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B21" t="str">
-        <v>3.10.2020, 21:14:1</v>
-      </c>
-      <c r="C21" t="str">
-        <v>3.10.2020, 21:15:4</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B22" t="str">
-        <v>3.10.2020, 21:16:8</v>
-      </c>
-      <c r="C22" t="str">
-        <v>3.10.2020, 21:16:13</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B23" t="str">
-        <v>3.10.2020, 21:16:24</v>
-      </c>
-      <c r="C23" t="str">
-        <v>3.10.2020, 21:16:34</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B24" t="str">
-        <v>3.10.2020, 21:16:37</v>
-      </c>
-      <c r="C24" t="str">
-        <v>3.10.2020, 21:16:41</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B25" t="str">
-        <v>3.10.2020, 21:17:8</v>
-      </c>
-      <c r="C25" t="str">
-        <v>3.10.2020, 21:17:12</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B26" t="str">
-        <v>3.10.2020, 21:18:16</v>
-      </c>
-      <c r="C26" t="str">
-        <v>3.10.2020, 21:19:0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B27" t="str">
-        <v>3.10.2020, 21:19:5</v>
-      </c>
-      <c r="C27" t="str">
-        <v>3.10.2020, 21:20:10</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B28" t="str">
-        <v>3.10.2020, 21:20:20</v>
-      </c>
-      <c r="C28" t="str">
-        <v>3.10.2020, 21:21:3</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="str">
-        <v>jane01 (cu dwawdd)</v>
-      </c>
-      <c r="B29" t="str">
-        <v>3.10.2020, 21:21:12</v>
-      </c>
-      <c r="C29" t="str">
-        <v>3.10.2020, 21:23:27</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="str">
-        <v>jane01 (cu ddd)</v>
-      </c>
-      <c r="B30" t="str">
-        <v>3.10.2020, 21:23:30</v>
-      </c>
-      <c r="C30" t="str">
-        <v>3.10.2020, 21:23:35</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B31" t="str">
-        <v>3.10.2020, 21:23:52</v>
-      </c>
-      <c r="C31" t="str">
-        <v>3.10.2020, 21:23:57</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="str">
-        <v>jane01</v>
-      </c>
-      <c r="B32" t="str">
-        <v>3.10.2020, 21:27:1</v>
-      </c>
-      <c r="C32" t="str">
-        <v>3.10.2020, 21:28:9</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="str">
-        <v>salexandru (cu Alex)</v>
-      </c>
-      <c r="B33" t="str">
-        <v>3.10.2020, 21:27:18</v>
-      </c>
-      <c r="C33" t="str">
-        <v>3.10.2020, 21:27:28</v>
+        <v>6.10.2020, 20:12:13</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C33"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C14"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>